<commit_message>
Hotfix on Mastertable and new ontology-md-files
</commit_message>
<xml_diff>
--- a/master_table/Possible_Template_TF_OntoWorldMap_2023-05-17-14-56_HB.xlsx
+++ b/master_table/Possible_Template_TF_OntoWorldMap_2023-05-17-14-56_HB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="21456" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="21456" firstSheet="7" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Template mit Beispiel" sheetId="4" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="453">
   <si>
     <t>Ontology</t>
   </si>
@@ -5640,8 +5640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5757,6 +5757,11 @@
         <v>452</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="62" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>21</v>
@@ -5835,6 +5840,11 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -6111,8 +6121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6271,9 +6281,19 @@
         <v>27</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -6580,8 +6600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A128"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6610,6 +6630,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>5</v>
@@ -6681,7 +6706,9 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
@@ -6771,6 +6798,11 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -7112,8 +7144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A128"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7193,7 +7225,9 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
@@ -7201,7 +7235,9 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
@@ -7209,7 +7245,9 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
@@ -7217,7 +7255,9 @@
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="71"/>
+      <c r="A23" s="71" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
@@ -7249,6 +7289,11 @@
         <v>25</v>
       </c>
     </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>27</v>
@@ -7294,9 +7339,19 @@
         <v>32</v>
       </c>
     </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -8557,8 +8612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8587,6 +8642,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>5</v>
@@ -8648,7 +8708,9 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
@@ -8656,7 +8718,9 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
@@ -8746,6 +8810,11 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -9082,8 +9151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A128"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9112,11 +9181,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>7</v>
@@ -9188,7 +9267,9 @@
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="71"/>
+      <c r="A23" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="25" spans="1:1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
@@ -9268,6 +9349,11 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -10136,7 +10222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -12962,6 +13048,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x010100E35C4A3F015220429587A6885988F55A" ma:contentTypeVersion="2" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="d6504310574d90ff3af330d88d4b27c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43c33c4e-3078-430a-a993-ec9e07a267b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7023e3b9e2c813b12cebe0f0ea1d5cce" ns2:_="">
     <xsd:import namespace="43c33c4e-3078-430a-a993-ec9e07a267b1"/>
@@ -13093,12 +13185,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E38D5B-D85B-4D43-8837-BDE8BD7F5B8A}">
   <ds:schemaRefs>
@@ -13108,6 +13194,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3709C412-EE61-448D-9135-2444D463CA94}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13123,13 +13218,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>